<commit_message>
Integrated all module and running error free
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCaseData.xlsx
+++ b/src/test/resources/TestCaseData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14794\eclipse-workspace\Dsalgoxpathers\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375792B0-B4E5-46F4-A477-4E7FCAF61035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C17DF3A-D299-41B3-8FFA-44A0A1E0DC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{09C7315B-D825-4338-9B1D-AEC147ED2C6B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">code </t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>print</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA43B848-157E-4DAD-8DB9-D4FC678C6FC6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,6 +430,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>